<commit_message>
solved the mystery of why I couldn't match pure python results in vscode
</commit_message>
<xml_diff>
--- a/inst/extdata/synthetic_data.xlsx
+++ b/inst/extdata/synthetic_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Drafts/2022_OrdinalSuStaInExample/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\fxtas\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F2A2C19-08EE-8E4A-A2F1-66324313FCED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89AB3A52-C88C-49FF-BA9A-6A0C15CD432B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10760" yWindow="4260" windowWidth="27640" windowHeight="16940" xr2:uid="{F6D5D4B9-329A-0442-B0F0-B9EDAA20EE43}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F6D5D4B9-329A-0442-B0F0-B9EDAA20EE43}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="12">
   <si>
     <t>Category</t>
   </si>
@@ -63,6 +63,15 @@
   </si>
   <si>
     <t>Biomarker 5</t>
+  </si>
+  <si>
+    <t>Sex</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>Female</t>
   </si>
 </sst>
 </file>
@@ -118,9 +127,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -158,7 +167,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -264,7 +273,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -406,7 +415,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -414,15 +423,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3C9EE5B-0332-194B-8ACC-1D6DFB73C39C}">
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -430,53 +439,59 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>6</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>7</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="C2">
-        <v>1</v>
+      <c r="C2" t="s">
+        <v>10</v>
       </c>
       <c r="D2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="H2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
       </c>
-      <c r="C3">
-        <v>0</v>
+      <c r="C3" t="s">
+        <v>11</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -490,200 +505,227 @@
       <c r="G3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>
       </c>
-      <c r="C4">
-        <v>1</v>
+      <c r="C4" t="s">
+        <v>10</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G4">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
       <c r="B5" t="s">
         <v>2</v>
       </c>
-      <c r="C5">
-        <v>1</v>
+      <c r="C5" t="s">
+        <v>11</v>
       </c>
       <c r="D5">
         <v>1</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F5">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G5">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
       <c r="B6" t="s">
         <v>2</v>
       </c>
-      <c r="C6">
-        <v>1</v>
+      <c r="C6" t="s">
+        <v>10</v>
       </c>
       <c r="D6">
         <v>1</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G6">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
       <c r="B7" t="s">
         <v>2</v>
       </c>
-      <c r="C7">
-        <v>2</v>
+      <c r="C7" t="s">
+        <v>11</v>
       </c>
       <c r="D7">
         <v>2</v>
       </c>
       <c r="E7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
       <c r="B8" t="s">
         <v>2</v>
       </c>
-      <c r="C8">
-        <v>2</v>
+      <c r="C8" t="s">
+        <v>10</v>
       </c>
       <c r="D8">
         <v>2</v>
       </c>
       <c r="E8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F8">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+      <c r="H8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
       <c r="B9" t="s">
         <v>2</v>
       </c>
-      <c r="C9">
-        <v>2</v>
+      <c r="C9" t="s">
+        <v>11</v>
       </c>
       <c r="D9">
         <v>2</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F9">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
       <c r="B10" t="s">
         <v>2</v>
       </c>
-      <c r="C10">
-        <v>2</v>
+      <c r="C10" t="s">
+        <v>10</v>
       </c>
       <c r="D10">
         <v>2</v>
       </c>
       <c r="E10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F10">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G10">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+      <c r="H10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
       <c r="B11" t="s">
         <v>2</v>
       </c>
-      <c r="C11">
-        <v>1</v>
+      <c r="C11" t="s">
+        <v>11</v>
       </c>
       <c r="D11">
         <v>1</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F11">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G11">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="H11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
       <c r="B12" t="s">
         <v>2</v>
       </c>
-      <c r="C12">
-        <v>0</v>
+      <c r="C12" t="s">
+        <v>10</v>
       </c>
       <c r="D12">
         <v>0</v>
@@ -697,68 +739,77 @@
       <c r="G12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
       <c r="B13" t="s">
         <v>2</v>
       </c>
-      <c r="C13">
-        <v>1</v>
+      <c r="C13" t="s">
+        <v>11</v>
       </c>
       <c r="D13">
         <v>1</v>
       </c>
       <c r="E13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F13">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G13">
         <v>2</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
       <c r="B14" t="s">
         <v>2</v>
       </c>
-      <c r="C14">
-        <v>1</v>
+      <c r="C14" t="s">
+        <v>10</v>
       </c>
       <c r="D14">
         <v>1</v>
       </c>
       <c r="E14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F14">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G14">
         <v>2</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
       <c r="B15" t="s">
         <v>2</v>
       </c>
-      <c r="C15">
-        <v>1</v>
+      <c r="C15" t="s">
+        <v>11</v>
       </c>
       <c r="D15">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F15">
         <v>1</v>
@@ -766,108 +817,123 @@
       <c r="G15">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
       <c r="B16" t="s">
         <v>2</v>
       </c>
-      <c r="C16">
-        <v>2</v>
+      <c r="C16" t="s">
+        <v>10</v>
       </c>
       <c r="D16">
         <v>2</v>
       </c>
       <c r="E16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G16">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="H16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
       <c r="B17" t="s">
         <v>2</v>
       </c>
-      <c r="C17">
-        <v>2</v>
+      <c r="C17" t="s">
+        <v>11</v>
       </c>
       <c r="D17">
         <v>2</v>
       </c>
       <c r="E17">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="H17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>16</v>
       </c>
       <c r="B18" t="s">
         <v>2</v>
       </c>
-      <c r="C18">
-        <v>1</v>
+      <c r="C18" t="s">
+        <v>10</v>
       </c>
       <c r="D18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E18">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F18">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G18">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="H18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>17</v>
       </c>
       <c r="B19" t="s">
         <v>2</v>
       </c>
-      <c r="C19">
-        <v>1</v>
+      <c r="C19" t="s">
+        <v>11</v>
       </c>
       <c r="D19">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E19">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F19">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G19">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="H19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>18</v>
       </c>
       <c r="B20" t="s">
         <v>2</v>
       </c>
-      <c r="C20">
-        <v>1</v>
+      <c r="C20" t="s">
+        <v>10</v>
       </c>
       <c r="D20">
         <v>1</v>
@@ -879,41 +945,47 @@
         <v>1</v>
       </c>
       <c r="G20">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="H20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>19</v>
       </c>
       <c r="B21" t="s">
         <v>2</v>
       </c>
-      <c r="C21">
-        <v>2</v>
+      <c r="C21" t="s">
+        <v>11</v>
       </c>
       <c r="D21">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F21">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="H21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>20</v>
       </c>
       <c r="B22" t="s">
         <v>3</v>
       </c>
-      <c r="C22">
-        <v>0</v>
+      <c r="C22" t="s">
+        <v>10</v>
       </c>
       <c r="D22">
         <v>0</v>
@@ -922,47 +994,53 @@
         <v>0</v>
       </c>
       <c r="F22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>21</v>
       </c>
       <c r="B23" t="s">
         <v>3</v>
       </c>
-      <c r="C23">
-        <v>0</v>
+      <c r="C23" t="s">
+        <v>11</v>
       </c>
       <c r="D23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E23">
         <v>1</v>
       </c>
       <c r="F23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G23">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>22</v>
       </c>
       <c r="B24" t="s">
         <v>3</v>
       </c>
-      <c r="C24">
-        <v>1</v>
+      <c r="C24" t="s">
+        <v>10</v>
       </c>
       <c r="D24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E24">
         <v>0</v>
@@ -971,18 +1049,21 @@
         <v>0</v>
       </c>
       <c r="G24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="H24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>23</v>
       </c>
       <c r="B25" t="s">
         <v>3</v>
       </c>
-      <c r="C25">
-        <v>0</v>
+      <c r="C25" t="s">
+        <v>11</v>
       </c>
       <c r="D25">
         <v>0</v>
@@ -996,16 +1077,19 @@
       <c r="G25">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>24</v>
       </c>
       <c r="B26" t="s">
         <v>3</v>
       </c>
-      <c r="C26">
-        <v>0</v>
+      <c r="C26" t="s">
+        <v>10</v>
       </c>
       <c r="D26">
         <v>0</v>
@@ -1017,6 +1101,9 @@
         <v>0</v>
       </c>
       <c r="G26">
+        <v>0</v>
+      </c>
+      <c r="H26">
         <v>0</v>
       </c>
     </row>

</xml_diff>